<commit_message>
added titles to dataset
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="9">
   <si>
     <t>Setosa</t>
   </si>
@@ -31,6 +31,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Virginica</t>
+  </si>
+  <si>
+    <t>sepal_length</t>
+  </si>
+  <si>
+    <t>sepal_width</t>
+  </si>
+  <si>
+    <t>petal_length</t>
+  </si>
+  <si>
+    <t>petal_width</t>
+  </si>
+  <si>
+    <t>species</t>
   </si>
 </sst>
 </file>
@@ -378,41 +393,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B1" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="C1" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D1" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="C2" s="2">
         <v>1.4</v>
@@ -426,13 +444,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B3" s="2">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D3" s="2">
         <v>0.2</v>
@@ -443,13 +461,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="B4" s="2">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C4" s="2">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D4" s="2">
         <v>0.2</v>
@@ -460,13 +478,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B5" s="2">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="C5" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="2">
         <v>0.2</v>
@@ -477,16 +495,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>3.9</v>
+        <v>3.6</v>
       </c>
       <c r="C6" s="2">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="D6" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -494,16 +512,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4.5999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="B7" s="2">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="C7" s="2">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="D7" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -511,16 +529,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B8" s="2">
         <v>3.4</v>
       </c>
       <c r="C8" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D8" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -528,13 +546,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="C9" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="2">
         <v>0.2</v>
@@ -545,16 +563,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B10" s="2">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="C10" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D10" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -562,16 +580,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>5.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B11" s="2">
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="C11" s="2">
         <v>1.5</v>
       </c>
       <c r="D11" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -579,13 +597,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="B12" s="2">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="C12" s="2">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D12" s="2">
         <v>0.2</v>
@@ -599,13 +617,13 @@
         <v>4.8</v>
       </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="C13" s="2">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D13" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
@@ -613,13 +631,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="B14" s="2">
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="D14" s="2">
         <v>0.1</v>
@@ -630,16 +648,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>5.8</v>
+        <v>4.3</v>
       </c>
       <c r="B15" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D15" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -647,16 +665,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="B16" s="2">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -664,13 +682,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
       <c r="B17" s="2">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C17" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="D17" s="2">
         <v>0.4</v>
@@ -681,16 +699,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>5.0999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="B18" s="2">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="C18" s="2">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="D18" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
@@ -698,13 +716,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B19" s="2">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="C19" s="2">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="D19" s="2">
         <v>0.3</v>
@@ -715,13 +733,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="B20" s="2">
         <v>3.8</v>
       </c>
       <c r="C20" s="2">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="D20" s="2">
         <v>0.3</v>
@@ -732,16 +750,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B21" s="2">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="C21" s="2">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="D21" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E21" t="s">
         <v>0</v>
@@ -749,16 +767,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>5.0999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="B22" s="2">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="C22" s="2">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="D22" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -766,16 +784,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>4.5999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B23" s="2">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D23" s="2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -783,16 +801,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>5.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B24" s="2">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="C24" s="2">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
@@ -800,16 +818,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>4.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B25" s="2">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="C25" s="2">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="D25" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E25" t="s">
         <v>0</v>
@@ -817,13 +835,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="B26" s="2">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="C26" s="2">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="D26" s="2">
         <v>0.2</v>
@@ -837,13 +855,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2">
         <v>1.6</v>
       </c>
       <c r="D27" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E27" t="s">
         <v>0</v>
@@ -851,16 +869,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C28" s="2">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D28" s="2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E28" t="s">
         <v>0</v>
@@ -871,10 +889,10 @@
         <v>5.2</v>
       </c>
       <c r="B29" s="2">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="C29" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D29" s="2">
         <v>0.2</v>
@@ -885,13 +903,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>4.7</v>
+        <v>5.2</v>
       </c>
       <c r="B30" s="2">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="C30" s="2">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D30" s="2">
         <v>0.2</v>
@@ -902,10 +920,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="B31" s="2">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C31" s="2">
         <v>1.6</v>
@@ -919,16 +937,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="B32" s="2">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="C32" s="2">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D32" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
@@ -936,16 +954,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>5.2</v>
+        <v>5.4</v>
       </c>
       <c r="B33" s="2">
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
       </c>
       <c r="D33" s="2">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E33" t="s">
         <v>0</v>
@@ -953,16 +971,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>5.5</v>
+        <v>5.2</v>
       </c>
       <c r="B34" s="2">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C34" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D34" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E34" t="s">
         <v>0</v>
@@ -970,13 +988,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="B35" s="2">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="C35" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D35" s="2">
         <v>0.2</v>
@@ -987,13 +1005,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B36" s="2">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C36" s="2">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="D36" s="2">
         <v>0.2</v>
@@ -1004,13 +1022,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="C37" s="2">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D37" s="2">
         <v>0.2</v>
@@ -1021,16 +1039,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="B38" s="2">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="C38" s="2">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="D38" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E38" t="s">
         <v>0</v>
@@ -1038,16 +1056,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B39" s="2">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="C39" s="2">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="D39" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E39" t="s">
         <v>0</v>
@@ -1055,13 +1073,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>5.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B40" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D40" s="2">
         <v>0.2</v>
@@ -1072,16 +1090,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B41" s="2">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C41" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="D41" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E41" t="s">
         <v>0</v>
@@ -1089,10 +1107,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
-        <v>2.2999999999999998</v>
+        <v>3.5</v>
       </c>
       <c r="C42" s="2">
         <v>1.3</v>
@@ -1106,16 +1124,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="B43" s="2">
-        <v>3.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C43" s="2">
         <v>1.3</v>
       </c>
       <c r="D43" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E43" t="s">
         <v>0</v>
@@ -1123,16 +1141,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B44" s="2">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="C44" s="2">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="D44" s="2">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="E44" t="s">
         <v>0</v>
@@ -1140,16 +1158,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="C45" s="2">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="D45" s="2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E45" t="s">
         <v>0</v>
@@ -1157,16 +1175,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>4.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B46" s="2">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="C46" s="2">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="D46" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E46" t="s">
         <v>0</v>
@@ -1174,16 +1192,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="B47" s="2">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D47" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E47" t="s">
         <v>0</v>
@@ -1191,13 +1209,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>4.5999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B48" s="2">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="C48" s="2">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D48" s="2">
         <v>0.2</v>
@@ -1208,13 +1226,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>5.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B49" s="2">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="C49" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D49" s="2">
         <v>0.2</v>
@@ -1225,13 +1243,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>5</v>
+        <v>5.3</v>
       </c>
       <c r="B50" s="2">
-        <v>3.3</v>
+        <v>3.7</v>
       </c>
       <c r="C50" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="D50" s="2">
         <v>0.2</v>
@@ -1242,33 +1260,33 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B51" s="2">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C51" s="2">
-        <v>4.7</v>
+        <v>1.4</v>
       </c>
       <c r="D51" s="2">
-        <v>1.4</v>
+        <v>0.2</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="B52" s="2">
         <v>3.2</v>
       </c>
       <c r="C52" s="2">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="D52" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E52" t="s">
         <v>1</v>
@@ -1276,13 +1294,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="B53" s="2">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C53" s="2">
-        <v>4.9000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="D53" s="2">
         <v>1.5</v>
@@ -1293,16 +1311,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>5.5</v>
+        <v>6.9</v>
       </c>
       <c r="B54" s="2">
-        <v>2.2999999999999998</v>
+        <v>3.1</v>
       </c>
       <c r="C54" s="2">
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D54" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
@@ -1310,16 +1328,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="B55" s="2">
-        <v>2.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C55" s="2">
-        <v>4.5999999999999996</v>
+        <v>4</v>
       </c>
       <c r="D55" s="2">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
@@ -1327,16 +1345,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>5.7</v>
+        <v>6.5</v>
       </c>
       <c r="B56" s="2">
         <v>2.8</v>
       </c>
       <c r="C56" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D56" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
@@ -1344,16 +1362,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="B57" s="2">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="C57" s="2">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="D57" s="2">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="E57" t="s">
         <v>1</v>
@@ -1361,16 +1379,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>4.9000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="B58" s="2">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="C58" s="2">
-        <v>3.3</v>
+        <v>4.7</v>
       </c>
       <c r="D58" s="2">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E58" t="s">
         <v>1</v>
@@ -1378,16 +1396,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>6.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B59" s="2">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="C59" s="2">
-        <v>4.5999999999999996</v>
+        <v>3.3</v>
       </c>
       <c r="D59" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
         <v>1</v>
@@ -1395,16 +1413,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>5.2</v>
+        <v>6.6</v>
       </c>
       <c r="B60" s="2">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="C60" s="2">
-        <v>3.9</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D60" s="2">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E60" t="s">
         <v>1</v>
@@ -1412,16 +1430,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="B61" s="2">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="C61" s="2">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="D61" s="2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="E61" t="s">
         <v>1</v>
@@ -1429,16 +1447,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>5.9</v>
+        <v>5</v>
       </c>
       <c r="B62" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="2">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="D62" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
         <v>1</v>
@@ -1446,16 +1464,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="B63" s="2">
-        <v>2.2000000000000002</v>
+        <v>3</v>
       </c>
       <c r="C63" s="2">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="D63" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E63" t="s">
         <v>1</v>
@@ -1463,16 +1481,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="B64" s="2">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C64" s="2">
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
         <v>1</v>
@@ -1480,16 +1498,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="B65" s="2">
         <v>2.9</v>
       </c>
       <c r="C65" s="2">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
       <c r="D65" s="2">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E65" t="s">
         <v>1</v>
@@ -1497,16 +1515,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>6.7</v>
+        <v>5.6</v>
       </c>
       <c r="B66" s="2">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="C66" s="2">
-        <v>4.4000000000000004</v>
+        <v>3.6</v>
       </c>
       <c r="D66" s="2">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E66" t="s">
         <v>1</v>
@@ -1514,16 +1532,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>5.6</v>
+        <v>6.7</v>
       </c>
       <c r="B67" s="2">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C67" s="2">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D67" s="2">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E67" t="s">
         <v>1</v>
@@ -1531,16 +1549,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="B68" s="2">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="C68" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="D68" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E68" t="s">
         <v>1</v>
@@ -1548,16 +1566,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
       <c r="B69" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="C69" s="2">
-        <v>4.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D69" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
         <v>1</v>
@@ -1565,16 +1583,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>5.6</v>
+        <v>6.2</v>
       </c>
       <c r="B70" s="2">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C70" s="2">
-        <v>3.9</v>
+        <v>4.5</v>
       </c>
       <c r="D70" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="E70" t="s">
         <v>1</v>
@@ -1582,16 +1600,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>5.9</v>
+        <v>5.6</v>
       </c>
       <c r="B71" s="2">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C71" s="2">
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
       <c r="D71" s="2">
-        <v>1.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E71" t="s">
         <v>1</v>
@@ -1599,16 +1617,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B72" s="2">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="C72" s="2">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="D72" s="2">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
       <c r="E72" t="s">
         <v>1</v>
@@ -1616,16 +1634,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="B73" s="2">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="C73" s="2">
-        <v>4.9000000000000004</v>
+        <v>4</v>
       </c>
       <c r="D73" s="2">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E73" t="s">
         <v>1</v>
@@ -1633,16 +1651,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="B74" s="2">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="C74" s="2">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D74" s="2">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="E74" t="s">
         <v>1</v>
@@ -1650,16 +1668,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="B75" s="2">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="C75" s="2">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="D75" s="2">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E75" t="s">
         <v>1</v>
@@ -1667,16 +1685,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="B76" s="2">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="C76" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="D76" s="2">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E76" t="s">
         <v>1</v>
@@ -1684,13 +1702,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="B77" s="2">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C77" s="2">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D77" s="2">
         <v>1.4</v>
@@ -1701,16 +1719,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="B78" s="2">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C78" s="2">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="D78" s="2">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="E78" t="s">
         <v>1</v>
@@ -1718,16 +1736,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>6</v>
+        <v>6.7</v>
       </c>
       <c r="B79" s="2">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="C79" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D79" s="2">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E79" t="s">
         <v>1</v>
@@ -1735,16 +1753,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="2">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="C80" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="D80" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E80" t="s">
         <v>1</v>
@@ -1752,16 +1770,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="B81" s="2">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="C81" s="2">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="D81" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E81" t="s">
         <v>1</v>
@@ -1775,10 +1793,10 @@
         <v>2.4</v>
       </c>
       <c r="C82" s="2">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="D82" s="2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E82" t="s">
         <v>1</v>
@@ -1786,16 +1804,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>5.8</v>
+        <v>5.5</v>
       </c>
       <c r="B83" s="2">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="C83" s="2">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="D83" s="2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
         <v>1</v>
@@ -1803,16 +1821,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>6</v>
+        <v>5.8</v>
       </c>
       <c r="B84" s="2">
         <v>2.7</v>
       </c>
       <c r="C84" s="2">
-        <v>5.0999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="D84" s="2">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="E84" t="s">
         <v>1</v>
@@ -1820,16 +1838,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>5.4</v>
+        <v>6</v>
       </c>
       <c r="B85" s="2">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C85" s="2">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D85" s="2">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="E85" t="s">
         <v>1</v>
@@ -1837,16 +1855,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="B86" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C86" s="2">
         <v>4.5</v>
       </c>
       <c r="D86" s="2">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E86" t="s">
         <v>1</v>
@@ -1854,16 +1872,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>6.7</v>
+        <v>6</v>
       </c>
       <c r="B87" s="2">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="C87" s="2">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="D87" s="2">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="E87" t="s">
         <v>1</v>
@@ -1871,16 +1889,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>6.3</v>
+        <v>6.7</v>
       </c>
       <c r="B88" s="2">
-        <v>2.2999999999999998</v>
+        <v>3.1</v>
       </c>
       <c r="C88" s="2">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="D88" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E88" t="s">
         <v>1</v>
@@ -1888,13 +1906,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>5.6</v>
+        <v>6.3</v>
       </c>
       <c r="B89" s="2">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C89" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D89" s="2">
         <v>1.3</v>
@@ -1905,13 +1923,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="B90" s="2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D90" s="2">
         <v>1.3</v>
@@ -1925,13 +1943,13 @@
         <v>5.5</v>
       </c>
       <c r="B91" s="2">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C91" s="2">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="D91" s="2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E91" t="s">
         <v>1</v>
@@ -1939,16 +1957,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>6.1</v>
+        <v>5.5</v>
       </c>
       <c r="B92" s="2">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C92" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D92" s="2">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="E92" t="s">
         <v>1</v>
@@ -1956,16 +1974,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="B93" s="2">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="C93" s="2">
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D93" s="2">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="E93" t="s">
         <v>1</v>
@@ -1973,16 +1991,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>5</v>
+        <v>5.8</v>
       </c>
       <c r="B94" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="C94" s="2">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="D94" s="2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E94" t="s">
         <v>1</v>
@@ -1990,16 +2008,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="B95" s="2">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C95" s="2">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="D95" s="2">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="E95" t="s">
         <v>1</v>
@@ -2007,16 +2025,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="B96" s="2">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C96" s="2">
         <v>4.2</v>
       </c>
       <c r="D96" s="2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E96" t="s">
         <v>1</v>
@@ -2027,13 +2045,13 @@
         <v>5.7</v>
       </c>
       <c r="B97" s="2">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="C97" s="2">
         <v>4.2</v>
       </c>
       <c r="D97" s="2">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E97" t="s">
         <v>1</v>
@@ -2041,13 +2059,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="B98" s="2">
         <v>2.9</v>
       </c>
       <c r="C98" s="2">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="D98" s="2">
         <v>1.3</v>
@@ -2058,16 +2076,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>5.0999999999999996</v>
+        <v>6.2</v>
       </c>
       <c r="B99" s="2">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="C99" s="2">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="D99" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="E99" t="s">
         <v>1</v>
@@ -2075,16 +2093,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B100" s="2">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="C100" s="2">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="D100" s="2">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E100" t="s">
         <v>1</v>
@@ -2092,33 +2110,33 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="B101" s="2">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="C101" s="2">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D101" s="2">
-        <v>2.5</v>
+        <v>1.3</v>
       </c>
       <c r="E101" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="B102" s="2">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="C102" s="2">
-        <v>5.0999999999999996</v>
+        <v>6</v>
       </c>
       <c r="D102" s="2">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="E102" t="s">
         <v>2</v>
@@ -2126,16 +2144,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
       <c r="B103" s="2">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C103" s="2">
-        <v>5.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D103" s="2">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="E103" t="s">
         <v>2</v>
@@ -2143,16 +2161,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>6.3</v>
+        <v>7.1</v>
       </c>
       <c r="B104" s="2">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="C104" s="2">
-        <v>5.6</v>
+        <v>5.9</v>
       </c>
       <c r="D104" s="2">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="E104" t="s">
         <v>2</v>
@@ -2160,16 +2178,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="B105" s="2">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="C105" s="2">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="D105" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="E105" t="s">
         <v>2</v>
@@ -2177,16 +2195,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>7.6</v>
+        <v>6.5</v>
       </c>
       <c r="B106" s="2">
         <v>3</v>
       </c>
       <c r="C106" s="2">
-        <v>6.6</v>
+        <v>5.8</v>
       </c>
       <c r="D106" s="2">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E106" t="s">
         <v>2</v>
@@ -2194,16 +2212,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>4.9000000000000004</v>
+        <v>7.6</v>
       </c>
       <c r="B107" s="2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C107" s="2">
-        <v>4.5</v>
+        <v>6.6</v>
       </c>
       <c r="D107" s="2">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="E107" t="s">
         <v>2</v>
@@ -2211,16 +2229,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>7.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B108" s="2">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="C108" s="2">
-        <v>6.3</v>
+        <v>4.5</v>
       </c>
       <c r="D108" s="2">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="E108" t="s">
         <v>2</v>
@@ -2228,13 +2246,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="B109" s="2">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="C109" s="2">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="D109" s="2">
         <v>1.8</v>
@@ -2245,16 +2263,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>7.2</v>
+        <v>6.7</v>
       </c>
       <c r="B110" s="2">
-        <v>3.6</v>
+        <v>2.5</v>
       </c>
       <c r="C110" s="2">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="D110" s="2">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="E110" t="s">
         <v>2</v>
@@ -2262,16 +2280,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>6.5</v>
+        <v>7.2</v>
       </c>
       <c r="B111" s="2">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="C111" s="2">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D111" s="2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E111" t="s">
         <v>2</v>
@@ -2279,16 +2297,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="B112" s="2">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="C112" s="2">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D112" s="2">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E112" t="s">
         <v>2</v>
@@ -2296,16 +2314,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="B113" s="2">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C113" s="2">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
       <c r="D113" s="2">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="E113" t="s">
         <v>2</v>
@@ -2313,16 +2331,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>5.7</v>
+        <v>6.8</v>
       </c>
       <c r="B114" s="2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C114" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="D114" s="2">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E114" t="s">
         <v>2</v>
@@ -2330,16 +2348,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="B115" s="2">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="C115" s="2">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="D115" s="2">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="E115" t="s">
         <v>2</v>
@@ -2347,16 +2365,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>6.4</v>
+        <v>5.8</v>
       </c>
       <c r="B116" s="2">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="C116" s="2">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D116" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="E116" t="s">
         <v>2</v>
@@ -2364,36 +2382,36 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="B117" s="2">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="C117" s="2">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
       <c r="D117" s="2">
-        <v>1.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E117" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>7.7</v>
+        <v>6.5</v>
       </c>
       <c r="B118" s="2">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="C118" s="2">
-        <v>6.7</v>
+        <v>5.5</v>
       </c>
       <c r="D118" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="E118" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2401,13 +2419,13 @@
         <v>7.7</v>
       </c>
       <c r="B119" s="2">
-        <v>2.6</v>
+        <v>3.8</v>
       </c>
       <c r="C119" s="2">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="D119" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E119" t="s">
         <v>2</v>
@@ -2415,16 +2433,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>6</v>
+        <v>7.7</v>
       </c>
       <c r="B120" s="2">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="C120" s="2">
-        <v>5</v>
+        <v>6.9</v>
       </c>
       <c r="D120" s="2">
-        <v>1.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E120" t="s">
         <v>2</v>
@@ -2432,16 +2450,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="B121" s="2">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C121" s="2">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="D121" s="2">
-        <v>2.2999999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="E121" t="s">
         <v>2</v>
@@ -2449,16 +2467,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>5.6</v>
+        <v>6.9</v>
       </c>
       <c r="B122" s="2">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="C122" s="2">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
       <c r="D122" s="2">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E122" t="s">
         <v>2</v>
@@ -2466,13 +2484,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>7.7</v>
+        <v>5.6</v>
       </c>
       <c r="B123" s="2">
         <v>2.8</v>
       </c>
       <c r="C123" s="2">
-        <v>6.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D123" s="2">
         <v>2</v>
@@ -2483,16 +2501,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>6.3</v>
+        <v>7.7</v>
       </c>
       <c r="B124" s="2">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="C124" s="2">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
       <c r="D124" s="2">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="E124" t="s">
         <v>2</v>
@@ -2500,16 +2518,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="B125" s="2">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="C125" s="2">
-        <v>5.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D125" s="2">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E125" t="s">
         <v>2</v>
@@ -2517,16 +2535,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>7.2</v>
+        <v>6.7</v>
       </c>
       <c r="B126" s="2">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C126" s="2">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="D126" s="2">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="E126" t="s">
         <v>2</v>
@@ -2534,13 +2552,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
       <c r="B127" s="2">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="C127" s="2">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="D127" s="2">
         <v>1.8</v>
@@ -2551,13 +2569,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="B128" s="2">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C128" s="2">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="D128" s="2">
         <v>1.8</v>
@@ -2568,16 +2586,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="B129" s="2">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C129" s="2">
-        <v>5.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D129" s="2">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E129" t="s">
         <v>2</v>
@@ -2585,16 +2603,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
       <c r="B130" s="2">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C130" s="2">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="D130" s="2">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="E130" t="s">
         <v>2</v>
@@ -2602,16 +2620,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="B131" s="2">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C131" s="2">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="D131" s="2">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="E131" t="s">
         <v>2</v>
@@ -2619,16 +2637,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>7.9</v>
+        <v>7.4</v>
       </c>
       <c r="B132" s="2">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="C132" s="2">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="D132" s="2">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="E132" t="s">
         <v>2</v>
@@ -2636,16 +2654,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="B133" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="C133" s="2">
         <v>6.4</v>
       </c>
-      <c r="B133" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="C133" s="2">
-        <v>5.6</v>
-      </c>
       <c r="D133" s="2">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="E133" t="s">
         <v>2</v>
@@ -2653,16 +2671,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="B134" s="2">
         <v>2.8</v>
       </c>
       <c r="C134" s="2">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D134" s="2">
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E134" t="s">
         <v>2</v>
@@ -2670,16 +2688,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="B135" s="2">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="C135" s="2">
-        <v>5.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D135" s="2">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E135" t="s">
         <v>2</v>
@@ -2687,16 +2705,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>7.7</v>
+        <v>6.1</v>
       </c>
       <c r="B136" s="2">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C136" s="2">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="D136" s="2">
-        <v>2.2999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="E136" t="s">
         <v>2</v>
@@ -2704,16 +2722,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>6.3</v>
+        <v>7.7</v>
       </c>
       <c r="B137" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C137" s="2">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="D137" s="2">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E137" t="s">
         <v>2</v>
@@ -2721,16 +2739,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="B138" s="2">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="C138" s="2">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="D138" s="2">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="E138" t="s">
         <v>2</v>
@@ -2738,13 +2756,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="B139" s="2">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C139" s="2">
-        <v>4.8</v>
+        <v>5.5</v>
       </c>
       <c r="D139" s="2">
         <v>1.8</v>
@@ -2755,16 +2773,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="B140" s="2">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="C140" s="2">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="D140" s="2">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E140" t="s">
         <v>2</v>
@@ -2772,16 +2790,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="B141" s="2">
         <v>3.1</v>
       </c>
       <c r="C141" s="2">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="D141" s="2">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="E141" t="s">
         <v>2</v>
@@ -2789,16 +2807,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="B142" s="2">
         <v>3.1</v>
       </c>
       <c r="C142" s="2">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D142" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="E142" t="s">
         <v>2</v>
@@ -2806,16 +2824,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>5.8</v>
+        <v>6.9</v>
       </c>
       <c r="B143" s="2">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="C143" s="2">
         <v>5.0999999999999996</v>
       </c>
       <c r="D143" s="2">
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E143" t="s">
         <v>2</v>
@@ -2823,16 +2841,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>6.8</v>
+        <v>5.8</v>
       </c>
       <c r="B144" s="2">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="C144" s="2">
-        <v>5.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D144" s="2">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="E144" t="s">
         <v>2</v>
@@ -2840,16 +2858,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="B145" s="2">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="C145" s="2">
-        <v>5.7</v>
+        <v>5.9</v>
       </c>
       <c r="D145" s="2">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E145" t="s">
         <v>2</v>
@@ -2860,13 +2878,13 @@
         <v>6.7</v>
       </c>
       <c r="B146" s="2">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="C146" s="2">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="D146" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="E146" t="s">
         <v>2</v>
@@ -2874,16 +2892,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>6.3</v>
+        <v>6.7</v>
       </c>
       <c r="B147" s="2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C147" s="2">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="D147" s="2">
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E147" t="s">
         <v>2</v>
@@ -2891,16 +2909,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="B148" s="2">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="C148" s="2">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="D148" s="2">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="E148" t="s">
         <v>2</v>
@@ -2908,16 +2926,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="B149" s="2">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="C149" s="2">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
       <c r="D149" s="2">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
       <c r="E149" t="s">
         <v>2</v>
@@ -2925,18 +2943,35 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="B150" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="C150" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="D150" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
         <v>5.9</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B151" s="2">
         <v>3</v>
       </c>
-      <c r="C150" s="2">
+      <c r="C151" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D150" s="2">
+      <c r="D151" s="2">
         <v>1.8</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E151" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added basic linear separability!
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>